<commit_message>
minor fixes in the code
</commit_message>
<xml_diff>
--- a/DHS7tabplan/DHS8-Module-FGCut-Tabplan-EN-24Apr2020-DHSQM.xlsx
+++ b/DHS7tabplan/DHS8-Module-FGCut-Tabplan-EN-24Apr2020-DHSQM.xlsx
@@ -7467,8 +7467,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="533" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ee862ef0fc8dbdbaa6c7a8968b7b48f1">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd4fdd4f38f705a4fbfd7d3200bf1970" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="534" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a765ce11b89b42bcade51542d07405">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f7cf592af29221d7e264e507c9f7a8c" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
     <xsd:import namespace="d16efad5-0601-4cf0-b7c2-89968258c777"/>
@@ -7496,6 +7496,7 @@
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -7581,6 +7582,11 @@
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="28" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -7738,10 +7744,10 @@
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <_dlc_DocId xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">VMX3MACP777Z-432858100-13994</_dlc_DocId>
+    <_dlc_DocId xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">VMX3MACP777Z-432858100-17731</_dlc_DocId>
     <_dlc_DocIdUrl xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">
-      <Url>https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/_layouts/15/DocIdRedir.aspx?ID=VMX3MACP777Z-432858100-13994</Url>
-      <Description>VMX3MACP777Z-432858100-13994</Description>
+      <Url>https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/_layouts/15/DocIdRedir.aspx?ID=VMX3MACP777Z-432858100-17731</Url>
+      <Description>VMX3MACP777Z-432858100-17731</Description>
     </_dlc_DocIdUrl>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <Survey_x0020_Type xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">DHS</Survey_x0020_Type>
@@ -7768,7 +7774,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50C1AAFB-60CC-4D25-B97F-6EF7CD7A32FF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48B7E365-260F-4888-81FD-E04F19C01E98}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Water and Sanitation variables moved to Chapter 16
</commit_message>
<xml_diff>
--- a/DHS7tabplan/DHS8-Module-FGCut-Tabplan-EN-24Apr2020-DHSQM.xlsx
+++ b/DHS7tabplan/DHS8-Module-FGCut-Tabplan-EN-24Apr2020-DHSQM.xlsx
@@ -7467,8 +7467,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="537" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="32af978db1d8a110ec558ab40ef27856">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" xmlns:ns4="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="490a248aacda82af6307d667c2e14f68" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="539" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e65afdd88d63c33e1d1950b49c9974fb">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" xmlns:ns4="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0fceb267320b0094ff995997203c92b4" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
     <xsd:import namespace="d16efad5-0601-4cf0-b7c2-89968258c777"/>
@@ -7500,6 +7500,8 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns4:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -7598,6 +7600,16 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="32" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="33" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d16efad5-0601-4cf0-b7c2-89968258c777" elementFormDefault="qualified">
@@ -7803,7 +7815,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54CA0FF1-5549-4D54-9788-E23BB1F28E9A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9829C94C-15B6-4CD9-845C-0A17AF5D756C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>